<commit_message>
expenditure for 4th and 5th, fule expense for 4th
</commit_message>
<xml_diff>
--- a/Bike Petrol.xlsx
+++ b/Bike Petrol.xlsx
@@ -240,6 +240,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -272,6 +275,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -302,6 +308,9 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -337,6 +346,10 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -368,6 +381,10 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -402,23 +419,6 @@
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -464,17 +464,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F44" totalsRowCount="1">
-  <autoFilter ref="A1:F43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F45" totalsRowCount="1">
+  <autoFilter ref="A1:F44"/>
   <tableColumns count="6">
-    <tableColumn id="4" name="DATE " dataDxfId="11" totalsRowDxfId="5"/>
-    <tableColumn id="11" name="AMOUNT" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="4">
-      <totalsRowFormula>SUM(B2:B43)</totalsRowFormula>
+    <tableColumn id="4" name="DATE " dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="11" name="AMOUNT" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+      <totalsRowFormula>SUM(B2:B44)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Price/Liter" dataDxfId="9" totalsRowDxfId="3"/>
-    <tableColumn id="2" name="PETROL(In liter)" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="3" name="KM runned" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="1" name="Mileage" dataDxfId="6" totalsRowDxfId="0"/>
+    <tableColumn id="5" name="Price/Liter" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="PETROL(In liter)" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="KM runned" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="1" name="Mileage" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -767,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,16 +1542,32 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="8">
-        <f>SUM(B2:B43)</f>
-        <v>20400</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="10"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>43255</v>
+      </c>
+      <c r="B44" s="3">
+        <v>500</v>
+      </c>
+      <c r="C44" s="3">
+        <v>79.83</v>
+      </c>
+      <c r="D44" s="4">
+        <v>6.26</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="8">
+        <f>SUM(B2:B44)</f>
+        <v>20900</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>